<commit_message>
Add non-working days section to calendar, update styles, and enhance functionality for displaying non-working days. Update script versions and improve contrast for badges. Remove unused environment block styles and adjust configuration for non-working days.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A527CC-177B-3845-91C2-70FA9FD24AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB51E2E4-CC78-6943-92BC-F3B9B6A6F5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="時程規劃" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>環境名稱</t>
   </si>
@@ -55,63 +55,73 @@
     <t>備注說明</t>
   </si>
   <si>
+    <t>資料轉換驗證與測試</t>
+  </si>
+  <si>
+    <t>需確認資料完整性</t>
+  </si>
+  <si>
+    <t>AP需與第一梯次版本一致</t>
+  </si>
+  <si>
+    <t>平行測試與系統切換驗證</t>
+  </si>
+  <si>
+    <t>平測環境首次資料</t>
+  </si>
+  <si>
+    <t>第二梯次資料更新</t>
+  </si>
+  <si>
+    <t>IT前置準備之1.永豐BSP確認接收日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT前置準備之2.永豐BSP DB倒檔</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT前置準備之3.永豐BSP AP確認</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>未開始</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>資轉驗證環境</t>
-  </si>
-  <si>
-    <t>資料轉換驗證與測試</t>
-  </si>
-  <si>
-    <t>第一梯次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平測切轉環境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>進行中</t>
-  </si>
-  <si>
-    <t>需確認資料完整性</t>
-  </si>
-  <si>
-    <t>第二梯次</t>
-  </si>
-  <si>
-    <t>待開始</t>
-  </si>
-  <si>
-    <t>AP需與第一梯次版本一致</t>
-  </si>
-  <si>
-    <t>平測切轉環境</t>
-  </si>
-  <si>
-    <t>平行測試與系統切換驗證</t>
-  </si>
-  <si>
-    <t>平測環境首次資料</t>
-  </si>
-  <si>
-    <t>第二梯次資料更新</t>
-  </si>
-  <si>
-    <t>IT前置準備之1.永豐BSP確認接收日</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IT前置準備之2.永豐BSP DB倒檔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IT前置準備之3.永豐BSP AP確認</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三梯次</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -488,7 +498,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -497,7 +507,7 @@
     <col min="2" max="2" width="32.3984375" customWidth="1"/>
     <col min="3" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="21.3984375" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="7" max="7" width="31.19921875" customWidth="1"/>
     <col min="8" max="8" width="18.796875" customWidth="1"/>
     <col min="9" max="9" width="19.796875" customWidth="1"/>
     <col min="10" max="10" width="21.19921875" customWidth="1"/>
@@ -542,24 +552,24 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3">
         <v>46037</v>
@@ -568,10 +578,10 @@
         <v>46042</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3">
         <v>45301</v>
@@ -583,25 +593,25 @@
         <v>46034</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3">
         <v>46038</v>
@@ -610,10 +620,10 @@
         <v>46040</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H3" s="3">
         <v>45301</v>
@@ -625,27 +635,27 @@
         <v>46034</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
         <v>46044</v>
@@ -654,10 +664,10 @@
         <v>46049</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H4" s="3">
         <v>45309</v>
@@ -669,7 +679,7 @@
         <v>46034</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
@@ -677,13 +687,13 @@
     </row>
     <row r="5" spans="1:14" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>46054</v>
@@ -692,10 +702,10 @@
         <v>46058</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H5" s="3">
         <v>45319</v>
@@ -707,27 +717,27 @@
         <v>46034</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3">
         <v>46061</v>
@@ -736,10 +746,10 @@
         <v>46065</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H6" s="3">
         <v>45327</v>
@@ -751,23 +761,23 @@
         <v>46034</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3">
         <v>46061</v>
@@ -776,10 +786,10 @@
         <v>46065</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H7" s="3">
         <v>45327</v>
@@ -791,10 +801,10 @@
         <v>46034</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>

</xml_diff>

<commit_message>
Implement settings panel for task bar field display configuration, enhance JavaScript cache management, and update styles for new settings button. Refactor task bar rendering logic to support dynamic field display based on user settings. Update configuration for Excel file path and add business date handling in data processing.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB51E2E4-CC78-6943-92BC-F3B9B6A6F5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F628663-ED72-3B44-9196-6D32F604EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>環境名稱</t>
   </si>
@@ -122,6 +122,10 @@
   </si>
   <si>
     <t>進行中</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>營業日</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -495,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -507,17 +511,17 @@
     <col min="2" max="2" width="32.3984375" customWidth="1"/>
     <col min="3" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="21.3984375" customWidth="1"/>
-    <col min="7" max="7" width="31.19921875" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" customWidth="1"/>
     <col min="8" max="8" width="18.796875" customWidth="1"/>
     <col min="9" max="9" width="19.796875" customWidth="1"/>
-    <col min="10" max="10" width="21.19921875" customWidth="1"/>
-    <col min="11" max="11" width="30" customWidth="1"/>
-    <col min="12" max="12" width="41.19921875" customWidth="1"/>
-    <col min="13" max="13" width="39.19921875" customWidth="1"/>
-    <col min="14" max="14" width="44.796875" customWidth="1"/>
+    <col min="10" max="11" width="21.19921875" customWidth="1"/>
+    <col min="12" max="12" width="30" customWidth="1"/>
+    <col min="13" max="13" width="41.19921875" customWidth="1"/>
+    <col min="14" max="14" width="39.19921875" customWidth="1"/>
+    <col min="15" max="15" width="44.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="25" customHeight="1">
+    <row r="1" spans="1:15" ht="25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,19 +553,22 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="20" customHeight="1">
+    <row r="2" spans="1:15" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -592,18 +599,21 @@
       <c r="J2" s="3">
         <v>46034</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="M2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="20" customHeight="1">
+    <row r="3" spans="1:15" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -634,20 +644,23 @@
       <c r="J3" s="3">
         <v>46034</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="M3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="20" customHeight="1">
+    <row r="4" spans="1:15" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -678,14 +691,17 @@
       <c r="J4" s="3">
         <v>46034</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="20" customHeight="1">
+    <row r="5" spans="1:15" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -716,20 +732,23 @@
       <c r="J5" s="3">
         <v>46034</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="O5" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" ht="20" customHeight="1">
+    <row r="6" spans="1:15" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -760,16 +779,19 @@
       <c r="J6" s="3">
         <v>46034</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="20" customHeight="1">
+    <row r="7" spans="1:15" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -800,14 +822,17 @@
       <c r="J7" s="3">
         <v>46034</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Enhance cache management in JavaScript, update environment purpose handling in data processing, and add meta tags for cache control in HTML. Improve logging for cache clearing and script version updates. Update configuration for environment-specific colors in settings.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,124 +8,229 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F628663-ED72-3B44-9196-6D32F604EC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C933F2-F232-3040-9622-5F0911B0B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="14180" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="時程規劃" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
+  <si>
+    <t>環境目的</t>
+  </si>
+  <si>
+    <t>驗證起日</t>
+  </si>
+  <si>
+    <t>驗證迄日</t>
+  </si>
+  <si>
+    <t>工作內容</t>
+  </si>
+  <si>
+    <t>狀態</t>
+  </si>
+  <si>
+    <t>資料基準日</t>
+  </si>
+  <si>
+    <t>京城封版日</t>
+  </si>
+  <si>
+    <t>京城傳送中介檔日</t>
+  </si>
+  <si>
+    <t>備注說明</t>
+  </si>
+  <si>
+    <t>IT前置準備之1.永豐BSP確認接收日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT前置準備之2.永豐BSP DB倒檔</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT前置準備之3.永豐BSP AP確認</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>未開始</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>已完成</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資轉驗證環境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平測切轉環境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>進行中</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>營業日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>執行梯次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第一次]USER資料驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第二次]USER資料驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第三次]USER資料驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第四次]USER資料驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第五次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第五次]USER資料驗證</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置資料轉換與修正調整及準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資轉-IT前置準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT前置準備-平測</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>切轉-IT前置準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第一次]切轉演練</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第二次]平行測試</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第二次]切轉演練</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第三次]平行測試</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第三次]切轉演練 - 擬真演練</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第四次]平行測試</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[第一次]平行測試</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>環境名稱</t>
-  </si>
-  <si>
-    <t>環境目的</t>
-  </si>
-  <si>
-    <t>執行梯次</t>
-  </si>
-  <si>
-    <t>驗證起日</t>
-  </si>
-  <si>
-    <t>驗證迄日</t>
-  </si>
-  <si>
-    <t>工作內容</t>
-  </si>
-  <si>
-    <t>狀態</t>
-  </si>
-  <si>
-    <t>資料基準日</t>
-  </si>
-  <si>
-    <t>京城封版日</t>
-  </si>
-  <si>
-    <t>京城傳送中介檔日</t>
-  </si>
-  <si>
-    <t>備注說明</t>
-  </si>
-  <si>
-    <t>資料轉換驗證與測試</t>
-  </si>
-  <si>
-    <t>需確認資料完整性</t>
-  </si>
-  <si>
-    <t>AP需與第一梯次版本一致</t>
-  </si>
-  <si>
-    <t>平行測試與系統切換驗證</t>
-  </si>
-  <si>
-    <t>平測環境首次資料</t>
-  </si>
-  <si>
-    <t>第二梯次資料更新</t>
-  </si>
-  <si>
-    <t>IT前置準備之1.永豐BSP確認接收日</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IT前置準備之2.永豐BSP DB倒檔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IT前置準備之3.永豐BSP AP確認</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OO</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一次</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二次</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三次</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>未開始</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>已完成</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>資轉驗證環境</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>平測切轉環境</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>進行中</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>營業日</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>資轉環境-前置資料轉換與修正調整及準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IT準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次資轉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二次資轉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次平測</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三次資轉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四次資轉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第五次資轉</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>擬真演練</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -499,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="156" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -523,79 +628,77 @@
   <sheetData>
     <row r="1" spans="1:15" ht="25" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3">
-        <v>46037</v>
+        <v>46119</v>
       </c>
       <c r="E2" s="3">
-        <v>46042</v>
+        <v>46129</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3">
-        <v>45301</v>
-      </c>
-      <c r="I2" s="3">
-        <v>46033</v>
-      </c>
+        <v>46066</v>
+      </c>
+      <c r="I2" s="3"/>
       <c r="J2" s="3">
         <v>46034</v>
       </c>
@@ -603,44 +706,42 @@
         <v>46034</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D3" s="3">
-        <v>46038</v>
+        <v>46132</v>
       </c>
       <c r="E3" s="3">
-        <v>46040</v>
+        <v>46143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3">
-        <v>45301</v>
-      </c>
-      <c r="I3" s="3">
-        <v>46033</v>
-      </c>
+        <v>46066</v>
+      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3">
         <v>46034</v>
       </c>
@@ -648,46 +749,42 @@
         <v>46034</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3">
-        <v>46044</v>
+        <v>46146</v>
       </c>
       <c r="E4" s="3">
-        <v>46049</v>
+        <v>46150</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3">
-        <v>45309</v>
-      </c>
-      <c r="I4" s="3">
-        <v>46032</v>
-      </c>
+        <v>46066</v>
+      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3">
         <v>46034</v>
       </c>
@@ -695,40 +792,42 @@
         <v>46034</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3">
-        <v>46054</v>
+        <v>46153</v>
       </c>
       <c r="E5" s="3">
-        <v>46058</v>
+        <v>46164</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3">
-        <v>45319</v>
-      </c>
-      <c r="I5" s="3">
-        <v>46031</v>
-      </c>
+        <v>46066</v>
+      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="3">
         <v>46034</v>
       </c>
@@ -736,46 +835,38 @@
         <v>46034</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3">
-        <v>46061</v>
+        <v>46146</v>
       </c>
       <c r="E6" s="3">
-        <v>46065</v>
+        <v>46150</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H6" s="3">
-        <v>45327</v>
-      </c>
-      <c r="I6" s="3">
-        <v>46032</v>
-      </c>
+        <v>46066</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3">
         <v>46034</v>
       </c>
@@ -783,56 +874,607 @@
         <v>46034</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3">
+        <v>46153</v>
+      </c>
+      <c r="E7" s="3">
+        <v>46164</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3">
+        <v>46066</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K7" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="20" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="3">
+        <v>46167</v>
+      </c>
+      <c r="E8" s="3">
+        <v>46171</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="3">
+        <v>46150</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K8" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="20" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>46174</v>
+      </c>
+      <c r="E9" s="3">
+        <v>46185</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3">
+        <v>46150</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K9" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="20" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3">
+        <v>46174</v>
+      </c>
+      <c r="E10" s="3">
+        <v>46178</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3">
+        <v>46136</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K10" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="20" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>46181</v>
+      </c>
+      <c r="E11" s="3">
+        <v>46185</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3">
+        <v>46136</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K11" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" ht="20" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="3">
+        <v>46195</v>
+      </c>
+      <c r="E12" s="3">
+        <v>46199</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="3">
+        <v>46191</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K12" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" ht="20" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3">
-        <v>46061</v>
-      </c>
-      <c r="E7" s="3">
-        <v>46065</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="3">
-        <v>45327</v>
-      </c>
-      <c r="I7" s="3">
-        <v>46032</v>
-      </c>
-      <c r="J7" s="3">
-        <v>46034</v>
-      </c>
-      <c r="K7" s="3">
-        <v>46034</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="D13" s="3">
+        <v>46202</v>
+      </c>
+      <c r="E13" s="3">
+        <v>46213</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3">
+        <v>46191</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K13" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" ht="20" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3">
+        <v>46202</v>
+      </c>
+      <c r="E14" s="3">
+        <v>46206</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="3">
+        <v>46171</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K14" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" ht="20" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="D15" s="3">
+        <v>46209</v>
+      </c>
+      <c r="E15" s="3">
+        <v>46213</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="3">
+        <v>46171</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K15" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" ht="20" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="3">
+        <v>46223</v>
+      </c>
+      <c r="E16" s="3">
+        <v>46226</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3">
+        <v>46199</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K16" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" ht="20" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3">
+        <v>46227</v>
+      </c>
+      <c r="E17" s="3">
+        <v>46228</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="3">
+        <v>46199</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K17" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" ht="20" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3">
+        <v>46237</v>
+      </c>
+      <c r="E18" s="3">
+        <v>46241</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="3">
+        <v>46220</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K18" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" ht="20" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3">
+        <v>46244</v>
+      </c>
+      <c r="E19" s="3">
+        <v>46248</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="3">
+        <v>46220</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K19" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15" ht="20" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="3">
+        <v>46255</v>
+      </c>
+      <c r="E20" s="3">
+        <v>46256</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3">
+        <v>46248</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K20" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Update CONFIG_GUIDE.md and EXCEL_FORMAT.md to enhance color configuration for environments, clarify environment purpose handling based on execution batches, and improve task display settings. Remove outdated README_EXAMPLE.md and streamline usage instructions in USAGE.md. Adjust HTML for cache management and update script versioning. Refactor JavaScript for improved task bar field display configuration and data processing logic.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C933F2-F232-3040-9622-5F0911B0B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD26896-600F-CA4A-9245-0FEACA4618C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="14180" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="49">
   <si>
     <t>環境目的</t>
   </si>
@@ -206,31 +206,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>第一次資轉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二次資轉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一次平測</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三次資轉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第四次資轉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第五次資轉</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>擬真演練</t>
+    <t>平測第一次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>擬真第一次</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>URL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>html://127.0.0.1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -604,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="156" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -623,10 +611,10 @@
     <col min="12" max="12" width="30" customWidth="1"/>
     <col min="13" max="13" width="41.19921875" customWidth="1"/>
     <col min="14" max="14" width="39.19921875" customWidth="1"/>
-    <col min="15" max="15" width="44.796875" customWidth="1"/>
+    <col min="15" max="16" width="44.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="25" customHeight="1">
+    <row r="1" spans="1:16" ht="25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -672,8 +660,11 @@
       <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="20" customHeight="1">
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -681,7 +672,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3">
         <v>46119</v>
@@ -715,8 +706,11 @@
         <v>12</v>
       </c>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" ht="20" customHeight="1">
+      <c r="P2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -758,8 +752,11 @@
         <v>12</v>
       </c>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="20" customHeight="1">
+      <c r="P3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -767,7 +764,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <v>46146</v>
@@ -801,8 +798,11 @@
         <v>12</v>
       </c>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" ht="20" customHeight="1">
+      <c r="P4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -840,8 +840,11 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" ht="20" customHeight="1">
+      <c r="P5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -849,7 +852,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3">
         <v>46146</v>
@@ -885,8 +888,11 @@
       <c r="O6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="20" customHeight="1">
+      <c r="P6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -930,8 +936,11 @@
       <c r="O7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="20" customHeight="1">
+      <c r="P7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -939,7 +948,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3">
         <v>46167</v>
@@ -973,8 +982,11 @@
         <v>12</v>
       </c>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" ht="20" customHeight="1">
+      <c r="P8" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1014,8 +1026,11 @@
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" ht="20" customHeight="1">
+      <c r="P9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1059,8 +1074,11 @@
       <c r="O10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="20" customHeight="1">
+      <c r="P10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1100,8 +1118,11 @@
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" ht="20" customHeight="1">
+      <c r="P11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1109,7 +1130,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3">
         <v>46195</v>
@@ -1143,8 +1164,11 @@
         <v>12</v>
       </c>
       <c r="O12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" ht="20" customHeight="1">
+      <c r="P12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1184,8 +1208,11 @@
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" ht="20" customHeight="1">
+      <c r="P13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1225,8 +1252,11 @@
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" ht="20" customHeight="1">
+      <c r="P14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1266,8 +1296,11 @@
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" ht="20" customHeight="1">
+      <c r="P15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
@@ -1275,7 +1308,7 @@
         <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D16" s="3">
         <v>46223</v>
@@ -1309,8 +1342,11 @@
         <v>12</v>
       </c>
       <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:15" ht="20" customHeight="1">
+      <c r="P16" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1350,8 +1386,11 @@
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-    </row>
-    <row r="18" spans="1:15" ht="20" customHeight="1">
+      <c r="P17" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1359,7 +1398,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D18" s="3">
         <v>46237</v>
@@ -1393,8 +1432,11 @@
         <v>12</v>
       </c>
       <c r="O18" s="2"/>
-    </row>
-    <row r="19" spans="1:15" ht="20" customHeight="1">
+      <c r="P18" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1434,8 +1476,11 @@
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-    </row>
-    <row r="20" spans="1:15" ht="20" customHeight="1">
+      <c r="P19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1475,6 +1520,9 @@
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
+      <c r="P20" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Implement multi-month display feature in calendar, enhancing layout and task rendering for multiple months. Update CSS for new styles and adjust JavaScript to support dynamic month handling and task bar rendering across multiple months. Modify configuration to allow setting the number of months displayed simultaneously.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD26896-600F-CA4A-9245-0FEACA4618C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DF8262-5E9F-A041-B2D9-5616BBA6ED8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="14180" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="50">
   <si>
     <t>環境目的</t>
   </si>
@@ -219,6 +219,10 @@
   </si>
   <si>
     <t>html://127.0.0.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試環境</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -592,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P20"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1080,25 +1084,25 @@
     </row>
     <row r="11" spans="1:16" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3">
-        <v>46181</v>
+        <v>46174</v>
       </c>
       <c r="E11" s="3">
-        <v>46185</v>
+        <v>46178</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H11" s="3">
         <v>46136</v>
@@ -1111,32 +1115,36 @@
         <v>46034</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="P11" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3">
-        <v>46195</v>
+        <v>46181</v>
       </c>
       <c r="E12" s="3">
-        <v>46199</v>
+        <v>46185</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
@@ -1145,7 +1153,7 @@
         <v>17</v>
       </c>
       <c r="H12" s="3">
-        <v>46191</v>
+        <v>46136</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3">
@@ -1155,14 +1163,12 @@
         <v>46034</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2" t="s">
         <v>48</v>
@@ -1170,19 +1176,19 @@
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <v>46202</v>
+        <v>46195</v>
       </c>
       <c r="E13" s="3">
-        <v>46213</v>
+        <v>46199</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>13</v>
@@ -1201,12 +1207,14 @@
         <v>46034</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
         <v>48</v>
@@ -1214,19 +1222,19 @@
     </row>
     <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D14" s="3">
         <v>46202</v>
       </c>
       <c r="E14" s="3">
-        <v>46206</v>
+        <v>46213</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
@@ -1235,7 +1243,7 @@
         <v>17</v>
       </c>
       <c r="H14" s="3">
-        <v>46171</v>
+        <v>46191</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3">
@@ -1245,7 +1253,7 @@
         <v>46034</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>12</v>
@@ -1261,16 +1269,16 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3">
-        <v>46209</v>
+        <v>46202</v>
       </c>
       <c r="E15" s="3">
-        <v>46213</v>
+        <v>46206</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
@@ -1289,7 +1297,7 @@
         <v>46034</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>12</v>
@@ -1302,19 +1310,19 @@
     </row>
     <row r="16" spans="1:16" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3">
-        <v>46223</v>
+        <v>46209</v>
       </c>
       <c r="E16" s="3">
-        <v>46226</v>
+        <v>46213</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
@@ -1323,7 +1331,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="3">
-        <v>46199</v>
+        <v>46171</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3">
@@ -1333,14 +1341,12 @@
         <v>46034</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2" t="s">
         <v>48</v>
@@ -1348,19 +1354,19 @@
     </row>
     <row r="17" spans="1:16" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D17" s="3">
-        <v>46227</v>
+        <v>46223</v>
       </c>
       <c r="E17" s="3">
-        <v>46228</v>
+        <v>46226</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
@@ -1379,12 +1385,14 @@
         <v>46034</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2" t="s">
         <v>48</v>
@@ -1392,19 +1400,19 @@
     </row>
     <row r="18" spans="1:16" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3">
-        <v>46237</v>
+        <v>46227</v>
       </c>
       <c r="E18" s="3">
-        <v>46241</v>
+        <v>46228</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -1413,7 +1421,7 @@
         <v>17</v>
       </c>
       <c r="H18" s="3">
-        <v>46220</v>
+        <v>46199</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3">
@@ -1423,14 +1431,12 @@
         <v>46034</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2" t="s">
         <v>48</v>
@@ -1438,19 +1444,19 @@
     </row>
     <row r="19" spans="1:16" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="3">
-        <v>46244</v>
+        <v>46237</v>
       </c>
       <c r="E19" s="3">
-        <v>46248</v>
+        <v>46241</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -1469,12 +1475,14 @@
         <v>46034</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N19" s="2"/>
+      <c r="N19" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2" t="s">
         <v>48</v>
@@ -1482,19 +1490,19 @@
     </row>
     <row r="20" spans="1:16" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D20" s="3">
-        <v>46255</v>
+        <v>46244</v>
       </c>
       <c r="E20" s="3">
-        <v>46256</v>
+        <v>46248</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>13</v>
@@ -1503,7 +1511,7 @@
         <v>17</v>
       </c>
       <c r="H20" s="3">
-        <v>46248</v>
+        <v>46220</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3">
@@ -1513,7 +1521,7 @@
         <v>46034</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>12</v>
@@ -1521,6 +1529,50 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="20" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>46255</v>
+      </c>
+      <c r="E21" s="3">
+        <v>46256</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="3">
+        <v>46248</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K21" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance calendar performance with virtual scrolling feature, allowing efficient rendering of visible date cells when task count is high. Update configuration for virtual scroll settings and buffer. Improve task display logic to support rendering tasks in day cells and across multiple months. Refactor CSS for better layout and responsiveness of legend items. Implement logging utility for better debugging and error handling throughout the application.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DF8262-5E9F-A041-B2D9-5616BBA6ED8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F20FB-4F8D-0A49-9B31-4449F4A9AD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="660" windowWidth="14180" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="24120" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="時程規劃" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="52">
   <si>
     <t>環境目的</t>
   </si>
@@ -223,6 +223,14 @@
   </si>
   <si>
     <t>測試環境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OO2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OO1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -596,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -731,7 +739,7 @@
         <v>46143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
@@ -762,22 +770,22 @@
     </row>
     <row r="4" spans="1:16" ht="20" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
-        <v>46146</v>
+        <v>46132</v>
       </c>
       <c r="E4" s="3">
-        <v>46150</v>
+        <v>46143</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
@@ -793,7 +801,7 @@
         <v>46034</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>12</v>
@@ -808,19 +816,19 @@
     </row>
     <row r="5" spans="1:16" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="3">
-        <v>46153</v>
+        <v>46146</v>
       </c>
       <c r="E5" s="3">
-        <v>46164</v>
+        <v>46150</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
@@ -839,10 +847,14 @@
         <v>46034</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
         <v>48</v>
@@ -850,19 +862,19 @@
     </row>
     <row r="6" spans="1:16" ht="20" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3">
-        <v>46146</v>
+        <v>46153</v>
       </c>
       <c r="E6" s="3">
-        <v>46150</v>
+        <v>46164</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
@@ -881,36 +893,30 @@
         <v>46034</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
       <c r="P6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3">
-        <v>46153</v>
+        <v>46146</v>
       </c>
       <c r="E7" s="3">
-        <v>46164</v>
+        <v>46150</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
@@ -929,7 +935,7 @@
         <v>46034</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>12</v>
@@ -946,19 +952,19 @@
     </row>
     <row r="8" spans="1:16" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3">
-        <v>46167</v>
+        <v>46153</v>
       </c>
       <c r="E8" s="3">
-        <v>46171</v>
+        <v>46164</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
@@ -967,7 +973,7 @@
         <v>18</v>
       </c>
       <c r="H8" s="3">
-        <v>46150</v>
+        <v>46066</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3">
@@ -977,7 +983,7 @@
         <v>46034</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>12</v>
@@ -985,32 +991,34 @@
       <c r="N8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="P8" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3">
-        <v>46174</v>
+        <v>46167</v>
       </c>
       <c r="E9" s="3">
-        <v>46185</v>
+        <v>46171</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H9" s="3">
         <v>46150</v>
@@ -1023,12 +1031,14 @@
         <v>46034</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
         <v>48</v>
@@ -1036,19 +1046,19 @@
     </row>
     <row r="10" spans="1:16" ht="20" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3">
         <v>46174</v>
       </c>
       <c r="E10" s="3">
-        <v>46178</v>
+        <v>46185</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
@@ -1057,7 +1067,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="3">
-        <v>46136</v>
+        <v>46150</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3">
@@ -1067,24 +1077,20 @@
         <v>46034</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>35</v>
@@ -1132,25 +1138,25 @@
     </row>
     <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3">
-        <v>46181</v>
+        <v>46174</v>
       </c>
       <c r="E12" s="3">
-        <v>46185</v>
+        <v>46178</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H12" s="3">
         <v>46136</v>
@@ -1163,32 +1169,36 @@
         <v>46034</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="N12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="P12" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3">
-        <v>46195</v>
+        <v>46181</v>
       </c>
       <c r="E13" s="3">
-        <v>46199</v>
+        <v>46185</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>13</v>
@@ -1197,7 +1207,7 @@
         <v>17</v>
       </c>
       <c r="H13" s="3">
-        <v>46191</v>
+        <v>46136</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3">
@@ -1207,14 +1217,12 @@
         <v>46034</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
         <v>48</v>
@@ -1222,19 +1230,19 @@
     </row>
     <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="3">
-        <v>46202</v>
+        <v>46195</v>
       </c>
       <c r="E14" s="3">
-        <v>46213</v>
+        <v>46199</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
@@ -1253,12 +1261,14 @@
         <v>46034</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="2"/>
+      <c r="N14" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2" t="s">
         <v>48</v>
@@ -1266,19 +1276,19 @@
     </row>
     <row r="15" spans="1:16" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D15" s="3">
         <v>46202</v>
       </c>
       <c r="E15" s="3">
-        <v>46206</v>
+        <v>46213</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
@@ -1287,7 +1297,7 @@
         <v>17</v>
       </c>
       <c r="H15" s="3">
-        <v>46171</v>
+        <v>46191</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3">
@@ -1297,7 +1307,7 @@
         <v>46034</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>12</v>
@@ -1313,16 +1323,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="3">
-        <v>46209</v>
+        <v>46202</v>
       </c>
       <c r="E16" s="3">
-        <v>46213</v>
+        <v>46206</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
@@ -1341,7 +1351,7 @@
         <v>46034</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>12</v>
@@ -1354,19 +1364,19 @@
     </row>
     <row r="17" spans="1:16" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D17" s="3">
-        <v>46223</v>
+        <v>46209</v>
       </c>
       <c r="E17" s="3">
-        <v>46226</v>
+        <v>46213</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
@@ -1375,7 +1385,7 @@
         <v>17</v>
       </c>
       <c r="H17" s="3">
-        <v>46199</v>
+        <v>46171</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3">
@@ -1385,14 +1395,12 @@
         <v>46034</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N17" s="2"/>
       <c r="O17" s="2"/>
       <c r="P17" s="2" t="s">
         <v>48</v>
@@ -1400,19 +1408,19 @@
     </row>
     <row r="18" spans="1:16" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D18" s="3">
-        <v>46227</v>
+        <v>46223</v>
       </c>
       <c r="E18" s="3">
-        <v>46228</v>
+        <v>46226</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -1431,12 +1439,14 @@
         <v>46034</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="2"/>
+      <c r="N18" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2" t="s">
         <v>48</v>
@@ -1444,19 +1454,19 @@
     </row>
     <row r="19" spans="1:16" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D19" s="3">
-        <v>46237</v>
+        <v>46227</v>
       </c>
       <c r="E19" s="3">
-        <v>46241</v>
+        <v>46228</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -1465,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="3">
-        <v>46220</v>
+        <v>46199</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3">
@@ -1475,14 +1485,12 @@
         <v>46034</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2" t="s">
         <v>48</v>
@@ -1490,19 +1498,19 @@
     </row>
     <row r="20" spans="1:16" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="3">
-        <v>46244</v>
+        <v>46237</v>
       </c>
       <c r="E20" s="3">
-        <v>46248</v>
+        <v>46241</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>13</v>
@@ -1521,12 +1529,14 @@
         <v>46034</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2" t="s">
         <v>48</v>
@@ -1534,19 +1544,19 @@
     </row>
     <row r="21" spans="1:16" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D21" s="3">
-        <v>46255</v>
+        <v>46244</v>
       </c>
       <c r="E21" s="3">
-        <v>46256</v>
+        <v>46248</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
@@ -1555,7 +1565,7 @@
         <v>17</v>
       </c>
       <c r="H21" s="3">
-        <v>46248</v>
+        <v>46220</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3">
@@ -1565,7 +1575,7 @@
         <v>46034</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>12</v>
@@ -1573,6 +1583,50 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="20" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3">
+        <v>46255</v>
+      </c>
+      <c r="E22" s="3">
+        <v>46256</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="3">
+        <v>46248</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3">
+        <v>46034</v>
+      </c>
+      <c r="K22" s="3">
+        <v>46034</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove unused configuration file for unimplemented features and update date references in documentation and code to reflect the year 2026. Enhance task display logic with modernized label styles and implement task limits for better organization. Update CSS for improved layout and responsiveness of task items. Add auto-resize functionality for calendar on window size changes.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F20FB-4F8D-0A49-9B31-4449F4A9AD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AD93E0-43E2-0043-9E75-3301872A6655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="24120" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
   <si>
     <t>環境目的</t>
   </si>
@@ -223,14 +223,6 @@
   </si>
   <si>
     <t>測試環境</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OO2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OO1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -606,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -739,7 +731,7 @@
         <v>46143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
@@ -785,7 +777,7 @@
         <v>46143</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Enhance calendar performance and layout by optimizing CSS for rendering efficiency and task bar adjustments. Implement dynamic height adjustments for task bars to prevent overlap, and introduce a mechanism for finalizing task bar positions post-rendering. Update JavaScript to support virtual scrolling and auto-enable features based on date cell count. Modify configuration settings for task bar height and virtual scrolling thresholds.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AD93E0-43E2-0043-9E75-3301872A6655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6662567-1F8F-B849-AE9E-DEB1C899E21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="24120" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="49">
   <si>
     <t>環境目的</t>
   </si>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>平測切轉環境</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>進行中</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -206,11 +202,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>平測第一次</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>擬真第一次</t>
+    <t>擬真</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -222,7 +214,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>測試環境</t>
+    <t>切轉上線環境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平行測試環境</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -596,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -620,13 +616,13 @@
   <sheetData>
     <row r="1" spans="1:16" ht="25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -650,7 +646,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -665,15 +661,15 @@
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="20" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
@@ -701,7 +697,7 @@
         <v>46034</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>12</v>
@@ -711,7 +707,7 @@
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="20" customHeight="1">
@@ -719,7 +715,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -747,7 +743,7 @@
         <v>46034</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>12</v>
@@ -757,7 +753,7 @@
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="20" customHeight="1">
@@ -765,7 +761,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -793,7 +789,7 @@
         <v>46034</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>12</v>
@@ -803,15 +799,15 @@
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="20" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -839,7 +835,7 @@
         <v>46034</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>12</v>
@@ -849,7 +845,7 @@
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="20" customHeight="1">
@@ -857,7 +853,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -885,25 +881,23 @@
         <v>46034</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="20" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="3">
         <v>46146</v>
       </c>
@@ -927,7 +921,7 @@
         <v>46034</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>12</v>
@@ -939,15 +933,15 @@
         <v>12</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="20" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
@@ -975,7 +969,7 @@
         <v>46034</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>12</v>
@@ -987,15 +981,15 @@
         <v>12</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="20" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1023,7 +1017,7 @@
         <v>46034</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>12</v>
@@ -1033,7 +1027,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="20" customHeight="1">
@@ -1041,7 +1035,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
@@ -1056,7 +1050,7 @@
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="3">
         <v>46150</v>
@@ -1069,7 +1063,7 @@
         <v>46034</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>12</v>
@@ -1077,15 +1071,15 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="20" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -1100,7 +1094,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="3">
         <v>46136</v>
@@ -1113,7 +1107,7 @@
         <v>46034</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>12</v>
@@ -1125,30 +1119,30 @@
         <v>12</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="20" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3">
-        <v>46174</v>
+        <v>46181</v>
       </c>
       <c r="E12" s="3">
-        <v>46178</v>
+        <v>46185</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H12" s="3">
         <v>46136</v>
@@ -1166,31 +1160,27 @@
       <c r="M12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
       <c r="P12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="20" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3">
-        <v>46181</v>
+        <v>46195</v>
       </c>
       <c r="E13" s="3">
-        <v>46185</v>
+        <v>46199</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>13</v>
@@ -1199,7 +1189,7 @@
         <v>17</v>
       </c>
       <c r="H13" s="3">
-        <v>46136</v>
+        <v>46191</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3">
@@ -1209,32 +1199,34 @@
         <v>46034</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="20" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3">
-        <v>46195</v>
+        <v>46202</v>
       </c>
       <c r="E14" s="3">
-        <v>46199</v>
+        <v>46213</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
@@ -1253,34 +1245,32 @@
         <v>46034</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="20" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3">
         <v>46202</v>
       </c>
       <c r="E15" s="3">
-        <v>46213</v>
+        <v>46206</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
@@ -1289,7 +1279,7 @@
         <v>17</v>
       </c>
       <c r="H15" s="3">
-        <v>46191</v>
+        <v>46171</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3">
@@ -1299,7 +1289,7 @@
         <v>46034</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>12</v>
@@ -1307,24 +1297,24 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="20" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3">
-        <v>46202</v>
+        <v>46209</v>
       </c>
       <c r="E16" s="3">
-        <v>46206</v>
+        <v>46213</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>13</v>
@@ -1351,24 +1341,24 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="20" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3">
-        <v>46209</v>
+        <v>46223</v>
       </c>
       <c r="E17" s="3">
-        <v>46213</v>
+        <v>46226</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>13</v>
@@ -1377,7 +1367,7 @@
         <v>17</v>
       </c>
       <c r="H17" s="3">
-        <v>46171</v>
+        <v>46199</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3">
@@ -1387,32 +1377,34 @@
         <v>46034</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="20" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3">
-        <v>46223</v>
+        <v>46227</v>
       </c>
       <c r="E18" s="3">
-        <v>46226</v>
+        <v>46228</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>13</v>
@@ -1431,34 +1423,32 @@
         <v>46034</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N18" s="2"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="20" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D19" s="3">
-        <v>46227</v>
+        <v>46237</v>
       </c>
       <c r="E19" s="3">
-        <v>46228</v>
+        <v>46241</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>13</v>
@@ -1467,7 +1457,7 @@
         <v>17</v>
       </c>
       <c r="H19" s="3">
-        <v>46199</v>
+        <v>46220</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3">
@@ -1477,32 +1467,34 @@
         <v>46034</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N19" s="2"/>
+      <c r="N19" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="20" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="3">
-        <v>46237</v>
+        <v>46244</v>
       </c>
       <c r="E20" s="3">
-        <v>46241</v>
+        <v>46248</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>13</v>
@@ -1521,34 +1513,32 @@
         <v>46034</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="20" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D21" s="3">
-        <v>46244</v>
+        <v>46255</v>
       </c>
       <c r="E21" s="3">
-        <v>46248</v>
+        <v>46256</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>13</v>
@@ -1557,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="H21" s="3">
-        <v>46220</v>
+        <v>46248</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3">
@@ -1567,7 +1557,7 @@
         <v>46034</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>12</v>
@@ -1575,51 +1565,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="20" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="3">
-        <v>46255</v>
-      </c>
-      <c r="E22" s="3">
-        <v>46256</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="3">
-        <v>46248</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3">
-        <v>46034</v>
-      </c>
-      <c r="K22" s="3">
-        <v>46034</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement horizontal task layout in calendar with dynamic task card creation. Update CSS for responsive task display and scrollbar styling. Modify JavaScript to handle multiple tasks in a horizontal view and adjust configuration settings for task information visibility.
</commit_message>
<xml_diff>
--- a/resource/範例_藍圖之對應時程環境規劃.xlsx
+++ b/resource/範例_藍圖之對應時程環境規劃.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shawn/Documents/Shawn/project_calendar/project_calendar/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6662567-1F8F-B849-AE9E-DEB1C899E21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE127B7-5BF1-214D-8708-232D076FC68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="660" windowWidth="24120" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="54">
   <si>
     <t>環境目的</t>
   </si>
@@ -219,6 +219,26 @@
   </si>
   <si>
     <t>平行測試環境</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平測-IT前置準備</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOOOO1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOOOO2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOXX1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OOXX2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -594,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -727,7 +747,7 @@
         <v>46143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
@@ -743,7 +763,7 @@
         <v>46034</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>12</v>
@@ -773,7 +793,7 @@
         <v>46143</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
@@ -789,7 +809,7 @@
         <v>46034</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>12</v>
@@ -895,7 +915,7 @@
         <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="3">

</xml_diff>